<commit_message>
clean datasets, add header image
</commit_message>
<xml_diff>
--- a/data/SexualMisconduct_clean.xlsx
+++ b/data/SexualMisconduct_clean.xlsx
@@ -1,49 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mio/Google Drive/MS1/Qualitativ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mio/Documents/GitHub/ms1-project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C276C4-5E3C-7041-9786-96787A944CA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB88260D-EA5B-984C-9F00-8151A15D4FCE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="400" yWindow="940" windowWidth="27640" windowHeight="16540" xr2:uid="{44998105-937C-0043-A5FC-ACAFDEAE5848}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$A$2:$A$42</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$B$2:$B$42</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$C$2:$C$42</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$D$2:$D$42</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$2:$B$42</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$C$42</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$D$2:$D$42</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$A$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$2:$A$42</definedName>
-  </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Year</t>
   </si>
@@ -86,12 +75,15 @@
   <si>
     <t>no action/ongoing</t>
   </si>
+  <si>
+    <t>Administration</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -230,7 +222,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>Sheet1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -251,7 +243,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$42</c:f>
+              <c:f>Sheet1!$F$2:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -383,7 +375,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$42</c:f>
+              <c:f>Sheet1!$G$2:$G$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -467,7 +459,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -488,7 +480,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$42</c:f>
+              <c:f>Sheet1!$F$2:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -620,7 +612,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$42</c:f>
+              <c:f>Sheet1!$H$2:$H$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -656,7 +648,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
+              <c:f>Sheet1!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -677,7 +669,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$42</c:f>
+              <c:f>Sheet1!$F$2:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -809,7 +801,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$42</c:f>
+              <c:f>Sheet1!$I$2:$I$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -869,7 +861,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>Sheet1!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -890,7 +882,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$42</c:f>
+              <c:f>Sheet1!$F$2:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1022,7 +1014,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$42</c:f>
+              <c:f>Sheet1!$J$2:$J$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1136,7 +1128,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>Sheet1!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1157,7 +1149,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$42</c:f>
+              <c:f>Sheet1!$F$2:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1289,7 +1281,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$42</c:f>
+              <c:f>Sheet1!$K$2:$K$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1379,7 +1371,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$1</c:f>
+              <c:f>Sheet1!$L$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1400,7 +1392,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$42</c:f>
+              <c:f>Sheet1!$F$2:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1532,7 +1524,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$42</c:f>
+              <c:f>Sheet1!$L$2:$L$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1589,7 +1581,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$1</c:f>
+              <c:f>Sheet1!$M$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1610,7 +1602,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$42</c:f>
+              <c:f>Sheet1!$F$2:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1742,7 +1734,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$2:$L$42</c:f>
+              <c:f>Sheet1!$M$2:$M$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -1847,7 +1839,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$1</c:f>
+              <c:f>Sheet1!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1868,7 +1860,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$42</c:f>
+              <c:f>Sheet1!$F$2:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -2000,7 +1992,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$2:$M$42</c:f>
+              <c:f>Sheet1!$N$2:$N$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -2129,7 +2121,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$1</c:f>
+              <c:f>Sheet1!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2150,7 +2142,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$42</c:f>
+              <c:f>Sheet1!$F$2:$F$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -2282,7 +2274,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$42</c:f>
+              <c:f>Sheet1!$O$2:$O$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -2459,7 +2451,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -3157,115 +3149,115 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="16">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="21">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="31">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="22">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="32">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="24">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>13</c:v>
-                </c:pt>
                 <c:pt idx="35">
-                  <c:v>25</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>34</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>32</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>39</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>83</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>87</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3282,7 +3274,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3440,7 +3432,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$42</c:f>
+              <c:f>Sheet1!$E$2:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
@@ -3671,7 +3663,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -4979,13 +4971,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>550237</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>41413</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>600176</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>118749</xdr:rowOff>
@@ -5015,13 +5007,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>629188</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>49371</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>679127</xdr:colOff>
       <xdr:row>65</xdr:row>
       <xdr:rowOff>155964</xdr:rowOff>
@@ -5351,15 +5343,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26332542-A283-F743-83ED-83677C25B0CA}">
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="O76" sqref="O76"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5370,47 +5362,50 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
         <f>SUM(B2:B43,C2:C43)</f>
-        <v>754</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1978</v>
       </c>
@@ -5421,32 +5416,35 @@
         <v>2</v>
       </c>
       <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1978</v>
       </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="2">
+      <c r="O2" s="2"/>
+      <c r="P2" s="2">
         <v>2</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1979</v>
       </c>
@@ -5457,32 +5455,35 @@
         <v>2</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1979</v>
       </c>
-      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="2">
+      <c r="O3" s="2"/>
+      <c r="P3" s="2">
         <v>2</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1980</v>
       </c>
@@ -5493,34 +5494,37 @@
         <v>3</v>
       </c>
       <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1980</v>
       </c>
-      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
       <c r="K4" s="2"/>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2">
-        <v>1</v>
-      </c>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2"/>
       <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
         <v>3</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1981</v>
       </c>
@@ -5531,32 +5535,35 @@
         <v>2</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1981</v>
       </c>
-      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2">
         <v>2</v>
       </c>
-      <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="2">
+      <c r="O5" s="2"/>
+      <c r="P5" s="2">
         <v>3</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1982</v>
       </c>
@@ -5564,25 +5571,25 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
         <v>4</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1982</v>
       </c>
-      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
       <c r="K6" s="2"/>
-      <c r="L6" s="2">
-        <v>1</v>
-      </c>
+      <c r="L6" s="2"/>
       <c r="M6" s="2">
         <v>1</v>
       </c>
@@ -5590,13 +5597,16 @@
         <v>1</v>
       </c>
       <c r="O6" s="2">
+        <v>1</v>
+      </c>
+      <c r="P6" s="2">
         <v>4</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1983</v>
       </c>
@@ -5607,34 +5617,37 @@
         <v>1</v>
       </c>
       <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>1983</v>
       </c>
-      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2">
-        <v>1</v>
-      </c>
+      <c r="L7" s="2"/>
       <c r="M7" s="2">
         <v>1</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2">
+      <c r="N7" s="2">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2">
         <v>3</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1984</v>
       </c>
@@ -5642,35 +5655,38 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>3</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>1984</v>
       </c>
-      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-      <c r="M8" s="2">
+      <c r="M8" s="2"/>
+      <c r="N8" s="2">
         <v>2</v>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2">
+      <c r="O8" s="2"/>
+      <c r="P8" s="2">
         <v>3</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1985</v>
       </c>
@@ -5681,30 +5697,33 @@
         <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
         <v>1985</v>
       </c>
-      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-      <c r="M9" s="2">
-        <v>1</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2">
-        <v>1</v>
-      </c>
-      <c r="P9">
+      <c r="M9" s="2"/>
+      <c r="N9" s="2">
+        <v>1</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1986</v>
       </c>
@@ -5712,35 +5731,38 @@
         <v>0</v>
       </c>
       <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
         <v>4</v>
       </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10">
+      <c r="F10">
         <v>1986</v>
       </c>
-      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="2">
-        <v>1</v>
-      </c>
+      <c r="L10" s="2"/>
       <c r="M10" s="2">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2">
         <v>3</v>
       </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2">
+      <c r="O10" s="2"/>
+      <c r="P10" s="2">
         <v>4</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:16" s="3" customFormat="1">
+    <row r="11" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1987</v>
       </c>
@@ -5748,35 +5770,38 @@
         <v>0</v>
       </c>
       <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
         <v>4</v>
       </c>
-      <c r="D11" s="3">
-        <v>4</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="F11" s="3">
         <v>1987</v>
       </c>
-      <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
-      <c r="M11" s="4">
+      <c r="M11" s="4"/>
+      <c r="N11" s="4">
         <v>3</v>
       </c>
-      <c r="N11" s="4">
-        <v>1</v>
-      </c>
       <c r="O11" s="4">
+        <v>1</v>
+      </c>
+      <c r="P11" s="4">
         <v>4</v>
       </c>
-      <c r="P11" s="3">
+      <c r="Q11" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1988</v>
       </c>
@@ -5786,35 +5811,38 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>0</v>
       </c>
       <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
         <v>1988</v>
       </c>
-      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2">
+      <c r="J12" s="2"/>
+      <c r="K12" s="2">
         <v>0</v>
       </c>
-      <c r="K12" s="2"/>
       <c r="L12" s="2"/>
-      <c r="M12" s="2">
-        <v>0</v>
-      </c>
+      <c r="M12" s="2"/>
       <c r="N12" s="2">
         <v>0</v>
       </c>
       <c r="O12" s="2">
         <v>0</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="2">
         <v>0</v>
       </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1989</v>
       </c>
@@ -5822,37 +5850,40 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13">
         <v>4</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>1989</v>
       </c>
-      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="J13" s="2">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
       <c r="L13" s="2"/>
-      <c r="M13" s="2">
-        <v>1</v>
-      </c>
+      <c r="M13" s="2"/>
       <c r="N13" s="2">
+        <v>1</v>
+      </c>
+      <c r="O13" s="2">
         <v>2</v>
       </c>
-      <c r="O13" s="2">
+      <c r="P13" s="2">
         <v>4</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1990</v>
       </c>
@@ -5862,35 +5893,38 @@
       <c r="C14">
         <v>7</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14">
         <v>8</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>1990</v>
       </c>
-      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2">
         <v>5</v>
       </c>
-      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
-      <c r="M14" s="2">
+      <c r="M14" s="2"/>
+      <c r="N14" s="2">
         <v>2</v>
       </c>
-      <c r="N14" s="2">
-        <v>1</v>
-      </c>
       <c r="O14" s="2">
+        <v>1</v>
+      </c>
+      <c r="P14" s="2">
         <v>8</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1991</v>
       </c>
@@ -5898,43 +5932,46 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
         <v>14</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>1991</v>
       </c>
-      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2">
+      <c r="I15" s="2"/>
+      <c r="J15" s="2">
         <v>2</v>
       </c>
-      <c r="J15" s="2">
+      <c r="K15" s="2">
         <v>3</v>
       </c>
-      <c r="K15" s="2">
-        <v>1</v>
-      </c>
       <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
         <v>2</v>
       </c>
-      <c r="M15" s="2">
+      <c r="N15" s="2">
         <v>4</v>
       </c>
-      <c r="N15" s="2">
+      <c r="O15" s="2">
         <v>2</v>
       </c>
-      <c r="O15" s="2">
+      <c r="P15" s="2">
         <v>14</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="3" customFormat="1">
+    <row r="16" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>1992</v>
       </c>
@@ -5942,41 +5979,44 @@
         <v>1</v>
       </c>
       <c r="C16" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D16" s="3">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3">
         <v>11</v>
       </c>
-      <c r="E16" s="3">
+      <c r="F16" s="3">
         <v>1992</v>
       </c>
-      <c r="F16" s="4">
-        <v>1</v>
-      </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4">
-        <v>1</v>
-      </c>
-      <c r="I16" s="4"/>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4">
+        <v>1</v>
+      </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="4">
+      <c r="L16" s="4"/>
+      <c r="M16" s="4">
         <v>2</v>
       </c>
-      <c r="M16" s="4">
+      <c r="N16" s="4">
         <v>5</v>
       </c>
-      <c r="N16" s="4">
+      <c r="O16" s="4">
         <v>2</v>
       </c>
-      <c r="O16" s="4">
+      <c r="P16" s="4">
         <v>11</v>
       </c>
-      <c r="P16" s="3">
+      <c r="Q16" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="3" customFormat="1">
+    <row r="17" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>1993</v>
       </c>
@@ -5984,41 +6024,44 @@
         <v>1</v>
       </c>
       <c r="C17" s="3">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D17" s="3">
+        <v>5</v>
+      </c>
+      <c r="E17" s="3">
         <v>14</v>
       </c>
-      <c r="E17" s="3">
+      <c r="F17" s="3">
         <v>1993</v>
       </c>
-      <c r="F17" s="4">
+      <c r="G17" s="4">
         <v>2</v>
       </c>
-      <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="4">
+      <c r="I17" s="4"/>
+      <c r="J17" s="4">
         <v>4</v>
       </c>
-      <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="4">
+      <c r="L17" s="4"/>
+      <c r="M17" s="4">
         <v>2</v>
       </c>
-      <c r="M17" s="4">
+      <c r="N17" s="4">
         <v>5</v>
       </c>
-      <c r="N17" s="4">
-        <v>1</v>
-      </c>
       <c r="O17" s="4">
+        <v>1</v>
+      </c>
+      <c r="P17" s="4">
         <v>14</v>
       </c>
-      <c r="P17" s="3">
+      <c r="Q17" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1994</v>
       </c>
@@ -6026,41 +6069,44 @@
         <v>5</v>
       </c>
       <c r="C18">
-        <v>9</v>
-      </c>
-      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="E18">
         <v>14</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>1994</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2">
+      <c r="G18" s="2"/>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2">
         <v>5</v>
       </c>
-      <c r="J18" s="2">
-        <v>1</v>
-      </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2">
+      <c r="K18" s="2">
+        <v>1</v>
+      </c>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2">
         <v>3</v>
       </c>
-      <c r="M18" s="2">
+      <c r="N18" s="2">
         <v>4</v>
       </c>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2">
+      <c r="O18" s="2"/>
+      <c r="P18" s="2">
         <v>14</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="3" customFormat="1">
+    <row r="19" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>1995</v>
       </c>
@@ -6068,41 +6114,44 @@
         <v>9</v>
       </c>
       <c r="C19" s="3">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D19" s="3">
+        <v>4</v>
+      </c>
+      <c r="E19" s="3">
         <v>22</v>
       </c>
-      <c r="E19" s="3">
+      <c r="F19" s="3">
         <v>1995</v>
       </c>
-      <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="4">
-        <v>4</v>
-      </c>
+      <c r="I19" s="4"/>
       <c r="J19" s="4">
         <v>4</v>
       </c>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4">
+      <c r="K19" s="4">
+        <v>4</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4">
         <v>5</v>
       </c>
-      <c r="M19" s="4">
+      <c r="N19" s="4">
         <v>8</v>
       </c>
-      <c r="N19" s="4">
-        <v>1</v>
-      </c>
       <c r="O19" s="4">
+        <v>1</v>
+      </c>
+      <c r="P19" s="4">
         <v>22</v>
       </c>
-      <c r="P19" s="3">
+      <c r="Q19" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1996</v>
       </c>
@@ -6112,43 +6161,46 @@
       <c r="C20">
         <v>10</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20">
         <v>13</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>1996</v>
       </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2">
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2">
         <v>3</v>
-      </c>
-      <c r="I20" s="2">
-        <v>2</v>
       </c>
       <c r="J20" s="2">
         <v>2</v>
       </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2">
-        <v>1</v>
-      </c>
+      <c r="K20" s="2">
+        <v>2</v>
+      </c>
+      <c r="L20" s="2"/>
       <c r="M20" s="2">
+        <v>1</v>
+      </c>
+      <c r="N20" s="2">
         <v>3</v>
       </c>
-      <c r="N20" s="2">
-        <v>1</v>
-      </c>
       <c r="O20" s="2">
+        <v>1</v>
+      </c>
+      <c r="P20" s="2">
         <v>13</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1997</v>
       </c>
@@ -6156,47 +6208,50 @@
         <v>7</v>
       </c>
       <c r="C21">
-        <v>12</v>
-      </c>
-      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21">
         <v>19</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>1997</v>
       </c>
-      <c r="F21" s="2">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2">
+      <c r="G21" s="2">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2">
         <v>2</v>
       </c>
-      <c r="I21" s="2">
+      <c r="J21" s="2">
         <v>3</v>
       </c>
-      <c r="J21" s="2">
+      <c r="K21" s="2">
         <v>2</v>
       </c>
-      <c r="K21" s="2">
-        <v>1</v>
-      </c>
       <c r="L21" s="2">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2">
         <v>2</v>
       </c>
-      <c r="M21" s="2">
+      <c r="N21" s="2">
         <v>6</v>
       </c>
-      <c r="N21" s="2">
+      <c r="O21" s="2">
         <v>2</v>
       </c>
-      <c r="O21" s="2">
+      <c r="P21" s="2">
         <v>19</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1998</v>
       </c>
@@ -6206,37 +6261,40 @@
       <c r="C22">
         <v>4</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22">
         <v>5</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>1998</v>
       </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2">
+        <v>1</v>
+      </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="2">
-        <v>1</v>
-      </c>
-      <c r="J22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2">
+        <v>1</v>
+      </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="2">
+      <c r="M22" s="2"/>
+      <c r="N22" s="2">
         <v>2</v>
       </c>
-      <c r="N22" s="2">
-        <v>1</v>
-      </c>
       <c r="O22" s="2">
+        <v>1</v>
+      </c>
+      <c r="P22" s="2">
         <v>5</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1999</v>
       </c>
@@ -6244,43 +6302,46 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>10</v>
-      </c>
-      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2</v>
+      </c>
+      <c r="E23">
         <v>11</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>1999</v>
       </c>
-      <c r="F23" s="2">
-        <v>1</v>
-      </c>
-      <c r="G23" s="2"/>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="2">
+      <c r="I23" s="2"/>
+      <c r="J23" s="2">
         <v>3</v>
       </c>
-      <c r="J23" s="2">
+      <c r="K23" s="2">
         <v>2</v>
       </c>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2">
-        <v>2</v>
-      </c>
+      <c r="L23" s="2"/>
       <c r="M23" s="2">
         <v>2</v>
       </c>
       <c r="N23" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O23" s="2">
+        <v>1</v>
+      </c>
+      <c r="P23" s="2">
         <v>11</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2000</v>
       </c>
@@ -6288,41 +6349,44 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>4</v>
-      </c>
-      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2</v>
+      </c>
+      <c r="E24">
         <v>7</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>2000</v>
       </c>
-      <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2">
-        <v>1</v>
-      </c>
+      <c r="H24" s="2"/>
       <c r="I24" s="2">
+        <v>1</v>
+      </c>
+      <c r="J24" s="2">
         <v>2</v>
       </c>
-      <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-      <c r="L24" s="2">
-        <v>1</v>
-      </c>
+      <c r="L24" s="2"/>
       <c r="M24" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N24" s="2">
         <v>2</v>
       </c>
       <c r="O24" s="2">
+        <v>2</v>
+      </c>
+      <c r="P24" s="2">
         <v>8</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2001</v>
       </c>
@@ -6330,39 +6394,42 @@
         <v>2</v>
       </c>
       <c r="C25">
-        <v>8</v>
-      </c>
-      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2</v>
+      </c>
+      <c r="E25">
         <v>10</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>2001</v>
       </c>
-      <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2">
+      <c r="J25" s="2"/>
+      <c r="K25" s="2">
         <v>3</v>
       </c>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2">
+      <c r="L25" s="2"/>
+      <c r="M25" s="2">
         <v>2</v>
       </c>
-      <c r="M25" s="2">
+      <c r="N25" s="2">
         <v>3</v>
       </c>
-      <c r="N25" s="2">
+      <c r="O25" s="2">
         <v>2</v>
       </c>
-      <c r="O25" s="2">
+      <c r="P25" s="2">
         <v>10</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="3" customFormat="1">
+    <row r="26" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>2002</v>
       </c>
@@ -6370,41 +6437,44 @@
         <v>3</v>
       </c>
       <c r="C26" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D26" s="3">
+        <v>4</v>
+      </c>
+      <c r="E26" s="3">
         <v>10</v>
       </c>
-      <c r="E26" s="3">
+      <c r="F26" s="3">
         <v>2002</v>
       </c>
-      <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="4">
-        <v>1</v>
-      </c>
+      <c r="I26" s="4"/>
       <c r="J26" s="4">
+        <v>1</v>
+      </c>
+      <c r="K26" s="4">
         <v>2</v>
       </c>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4">
+      <c r="L26" s="4"/>
+      <c r="M26" s="4">
         <v>2</v>
       </c>
-      <c r="M26" s="4">
+      <c r="N26" s="4">
         <v>4</v>
       </c>
-      <c r="N26" s="4">
-        <v>1</v>
-      </c>
       <c r="O26" s="4">
+        <v>1</v>
+      </c>
+      <c r="P26" s="4">
         <v>10</v>
       </c>
-      <c r="P26" s="3">
+      <c r="Q26" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2003</v>
       </c>
@@ -6412,27 +6482,27 @@
         <v>4</v>
       </c>
       <c r="C27">
-        <v>2</v>
-      </c>
-      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>2003</v>
       </c>
-      <c r="F27" s="2">
-        <v>1</v>
-      </c>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2">
+        <v>1</v>
+      </c>
       <c r="H27" s="2"/>
-      <c r="I27" s="2">
-        <v>1</v>
-      </c>
-      <c r="J27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2">
+        <v>1</v>
+      </c>
       <c r="K27" s="2"/>
-      <c r="L27" s="2">
-        <v>1</v>
-      </c>
+      <c r="L27" s="2"/>
       <c r="M27" s="2">
         <v>1</v>
       </c>
@@ -6440,13 +6510,16 @@
         <v>1</v>
       </c>
       <c r="O27" s="2">
+        <v>1</v>
+      </c>
+      <c r="P27" s="2">
         <v>6</v>
       </c>
-      <c r="P27">
+      <c r="Q27">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2004</v>
       </c>
@@ -6454,43 +6527,46 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <v>12</v>
-      </c>
-      <c r="D28">
+        <v>9</v>
+      </c>
+      <c r="D28" s="3">
+        <v>3</v>
+      </c>
+      <c r="E28">
         <v>13</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>2004</v>
       </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2">
-        <v>1</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2">
+      <c r="G28" s="2"/>
+      <c r="H28" s="2">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2">
         <v>3</v>
       </c>
-      <c r="J28" s="2">
+      <c r="K28" s="2">
         <v>2</v>
       </c>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2">
-        <v>3</v>
-      </c>
+      <c r="L28" s="2"/>
       <c r="M28" s="2">
         <v>3</v>
       </c>
       <c r="N28" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O28" s="2">
+        <v>1</v>
+      </c>
+      <c r="P28" s="2">
         <v>13</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2005</v>
       </c>
@@ -6498,43 +6574,46 @@
         <v>3</v>
       </c>
       <c r="C29">
-        <v>7</v>
-      </c>
-      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1</v>
+      </c>
+      <c r="E29">
         <v>10</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>2005</v>
       </c>
-      <c r="F29" s="2">
+      <c r="G29" s="2">
         <v>2</v>
       </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2">
-        <v>1</v>
-      </c>
+      <c r="H29" s="2"/>
       <c r="I29" s="2">
         <v>1</v>
       </c>
       <c r="J29" s="2">
         <v>1</v>
       </c>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2">
-        <v>1</v>
-      </c>
+      <c r="K29" s="2">
+        <v>1</v>
+      </c>
+      <c r="L29" s="2"/>
       <c r="M29" s="2">
+        <v>1</v>
+      </c>
+      <c r="N29" s="2">
         <v>4</v>
       </c>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2">
+      <c r="O29" s="2"/>
+      <c r="P29" s="2">
         <v>10</v>
       </c>
-      <c r="P29">
+      <c r="Q29">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="3" customFormat="1">
+    <row r="30" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>2006</v>
       </c>
@@ -6542,45 +6621,48 @@
         <v>3</v>
       </c>
       <c r="C30" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D30" s="3">
+        <v>5</v>
+      </c>
+      <c r="E30" s="3">
         <v>13</v>
       </c>
-      <c r="E30" s="3">
+      <c r="F30" s="3">
         <v>2006</v>
       </c>
-      <c r="F30" s="4">
-        <v>1</v>
-      </c>
-      <c r="G30" s="4"/>
+      <c r="G30" s="4">
+        <v>1</v>
+      </c>
       <c r="H30" s="4"/>
-      <c r="I30" s="4">
+      <c r="I30" s="4"/>
+      <c r="J30" s="4">
         <v>2</v>
       </c>
-      <c r="J30" s="4">
-        <v>1</v>
-      </c>
       <c r="K30" s="4">
         <v>1</v>
       </c>
       <c r="L30" s="4">
+        <v>1</v>
+      </c>
+      <c r="M30" s="4">
         <v>2</v>
       </c>
-      <c r="M30" s="4">
+      <c r="N30" s="4">
         <v>5</v>
       </c>
-      <c r="N30" s="4">
-        <v>1</v>
-      </c>
       <c r="O30" s="4">
+        <v>1</v>
+      </c>
+      <c r="P30" s="4">
         <v>13</v>
       </c>
-      <c r="P30" s="3">
+      <c r="Q30" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="3" customFormat="1">
+    <row r="31" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>2007</v>
       </c>
@@ -6588,17 +6670,17 @@
         <v>9</v>
       </c>
       <c r="C31" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D31" s="3">
+        <v>4</v>
+      </c>
+      <c r="E31" s="3">
         <v>21</v>
       </c>
-      <c r="E31" s="3">
+      <c r="F31" s="3">
         <v>2007</v>
       </c>
-      <c r="F31" s="4">
-        <v>1</v>
-      </c>
       <c r="G31" s="4">
         <v>1</v>
       </c>
@@ -6606,29 +6688,32 @@
         <v>1</v>
       </c>
       <c r="I31" s="4">
+        <v>1</v>
+      </c>
+      <c r="J31" s="4">
         <v>5</v>
       </c>
-      <c r="J31" s="4">
+      <c r="K31" s="4">
         <v>3</v>
       </c>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4">
-        <v>1</v>
-      </c>
+      <c r="L31" s="4"/>
       <c r="M31" s="4">
+        <v>1</v>
+      </c>
+      <c r="N31" s="4">
         <v>8</v>
       </c>
-      <c r="N31" s="4">
-        <v>1</v>
-      </c>
       <c r="O31" s="4">
+        <v>1</v>
+      </c>
+      <c r="P31" s="4">
         <v>21</v>
       </c>
-      <c r="P31" s="3">
+      <c r="Q31" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="3" customFormat="1">
+    <row r="32" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>2008</v>
       </c>
@@ -6636,45 +6721,48 @@
         <v>6</v>
       </c>
       <c r="C32" s="3">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D32" s="3">
+        <v>5</v>
+      </c>
+      <c r="E32" s="3">
         <v>22</v>
       </c>
-      <c r="E32" s="3">
+      <c r="F32" s="3">
         <v>2008</v>
       </c>
-      <c r="F32" s="4">
-        <v>1</v>
-      </c>
-      <c r="G32" s="4"/>
+      <c r="G32" s="4">
+        <v>1</v>
+      </c>
       <c r="H32" s="4"/>
-      <c r="I32" s="4">
+      <c r="I32" s="4"/>
+      <c r="J32" s="4">
         <v>6</v>
-      </c>
-      <c r="J32" s="4">
-        <v>2</v>
       </c>
       <c r="K32" s="4">
         <v>2</v>
       </c>
       <c r="L32" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M32" s="4">
+        <v>1</v>
+      </c>
+      <c r="N32" s="4">
         <v>9</v>
       </c>
-      <c r="N32" s="4">
-        <v>1</v>
-      </c>
       <c r="O32" s="4">
+        <v>1</v>
+      </c>
+      <c r="P32" s="4">
         <v>22</v>
       </c>
-      <c r="P32" s="3">
+      <c r="Q32" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="3" customFormat="1">
+    <row r="33" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>2009</v>
       </c>
@@ -6682,41 +6770,44 @@
         <v>5</v>
       </c>
       <c r="C33" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D33" s="3">
+        <v>2</v>
+      </c>
+      <c r="E33" s="3">
         <v>16</v>
       </c>
-      <c r="E33" s="3">
+      <c r="F33" s="3">
         <v>2009</v>
       </c>
-      <c r="F33" s="4">
+      <c r="G33" s="4">
         <v>4</v>
       </c>
-      <c r="G33" s="4"/>
       <c r="H33" s="4"/>
-      <c r="I33" s="4">
+      <c r="I33" s="4"/>
+      <c r="J33" s="4">
         <v>3</v>
       </c>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4">
+      <c r="K33" s="4"/>
+      <c r="L33" s="4">
         <v>2</v>
       </c>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4">
+      <c r="M33" s="4"/>
+      <c r="N33" s="4">
         <v>5</v>
       </c>
-      <c r="N33" s="4">
+      <c r="O33" s="4">
         <v>2</v>
       </c>
-      <c r="O33" s="4">
+      <c r="P33" s="4">
         <v>16</v>
       </c>
-      <c r="P33" s="3">
+      <c r="Q33" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="3" customFormat="1">
+    <row r="34" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>2010</v>
       </c>
@@ -6724,43 +6815,46 @@
         <v>2</v>
       </c>
       <c r="C34" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D34" s="3">
+        <v>2</v>
+      </c>
+      <c r="E34" s="3">
         <v>14</v>
       </c>
-      <c r="E34" s="3">
+      <c r="F34" s="3">
         <v>2010</v>
       </c>
-      <c r="F34" s="4">
+      <c r="G34" s="4">
         <v>2</v>
       </c>
-      <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="4">
+      <c r="I34" s="4"/>
+      <c r="J34" s="4">
         <v>4</v>
       </c>
-      <c r="J34" s="4">
+      <c r="K34" s="4">
         <v>2</v>
       </c>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4">
-        <v>1</v>
-      </c>
+      <c r="L34" s="4"/>
       <c r="M34" s="4">
+        <v>1</v>
+      </c>
+      <c r="N34" s="4">
         <v>2</v>
       </c>
-      <c r="N34" s="4">
+      <c r="O34" s="4">
         <v>3</v>
       </c>
-      <c r="O34" s="4">
+      <c r="P34" s="4">
         <v>14</v>
       </c>
-      <c r="P34" s="3">
+      <c r="Q34" s="3">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="3" customFormat="1">
+    <row r="35" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>2011</v>
       </c>
@@ -6768,45 +6862,48 @@
         <v>6</v>
       </c>
       <c r="C35" s="3">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D35" s="3">
+        <v>10</v>
+      </c>
+      <c r="E35" s="3">
         <v>28</v>
       </c>
-      <c r="E35" s="3">
+      <c r="F35" s="3">
         <v>2011</v>
       </c>
-      <c r="F35" s="4">
-        <v>1</v>
-      </c>
-      <c r="G35" s="4"/>
+      <c r="G35" s="4">
+        <v>1</v>
+      </c>
       <c r="H35" s="4"/>
-      <c r="I35" s="4">
+      <c r="I35" s="4"/>
+      <c r="J35" s="4">
         <v>3</v>
       </c>
-      <c r="J35" s="4">
+      <c r="K35" s="4">
         <v>6</v>
       </c>
-      <c r="K35" s="4">
-        <v>1</v>
-      </c>
       <c r="L35" s="4">
         <v>1</v>
       </c>
       <c r="M35" s="4">
+        <v>1</v>
+      </c>
+      <c r="N35" s="4">
         <v>13</v>
       </c>
-      <c r="N35" s="4">
+      <c r="O35" s="4">
         <v>3</v>
       </c>
-      <c r="O35" s="4">
+      <c r="P35" s="4">
         <v>28</v>
       </c>
-      <c r="P35" s="3">
+      <c r="Q35" s="3">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="3" customFormat="1">
+    <row r="36" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>2012</v>
       </c>
@@ -6814,45 +6911,48 @@
         <v>2</v>
       </c>
       <c r="C36" s="3">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D36" s="3">
+        <v>5</v>
+      </c>
+      <c r="E36" s="3">
         <v>15</v>
       </c>
-      <c r="E36" s="3">
+      <c r="F36" s="3">
         <v>2012</v>
       </c>
-      <c r="F36" s="4">
-        <v>1</v>
-      </c>
-      <c r="G36" s="4"/>
+      <c r="G36" s="4">
+        <v>1</v>
+      </c>
       <c r="H36" s="4"/>
-      <c r="I36" s="4">
-        <v>1</v>
-      </c>
+      <c r="I36" s="4"/>
       <c r="J36" s="4">
+        <v>1</v>
+      </c>
+      <c r="K36" s="4">
         <v>2</v>
       </c>
-      <c r="K36" s="4">
-        <v>1</v>
-      </c>
       <c r="L36" s="4">
         <v>1</v>
       </c>
       <c r="M36" s="4">
+        <v>1</v>
+      </c>
+      <c r="N36" s="4">
         <v>8</v>
       </c>
-      <c r="N36" s="4">
-        <v>1</v>
-      </c>
       <c r="O36" s="4">
+        <v>1</v>
+      </c>
+      <c r="P36" s="4">
         <v>15</v>
       </c>
-      <c r="P36" s="3">
+      <c r="Q36" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:16" s="3" customFormat="1">
+    <row r="37" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>2013</v>
       </c>
@@ -6860,43 +6960,46 @@
         <v>6</v>
       </c>
       <c r="C37" s="3">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D37" s="3">
+        <v>7</v>
+      </c>
+      <c r="E37" s="3">
         <v>31</v>
       </c>
-      <c r="E37" s="3">
+      <c r="F37" s="3">
         <v>2013</v>
       </c>
-      <c r="F37" s="4">
-        <v>1</v>
-      </c>
-      <c r="G37" s="4"/>
+      <c r="G37" s="4">
+        <v>1</v>
+      </c>
       <c r="H37" s="4"/>
-      <c r="I37" s="4">
+      <c r="I37" s="4"/>
+      <c r="J37" s="4">
         <v>10</v>
       </c>
-      <c r="J37" s="4">
+      <c r="K37" s="4">
         <v>2</v>
       </c>
-      <c r="K37" s="4">
-        <v>1</v>
-      </c>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4">
+      <c r="L37" s="4">
+        <v>1</v>
+      </c>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4">
         <v>12</v>
       </c>
-      <c r="N37" s="4">
+      <c r="O37" s="4">
         <v>5</v>
       </c>
-      <c r="O37" s="4">
+      <c r="P37" s="4">
         <v>31</v>
       </c>
-      <c r="P37" s="3">
+      <c r="Q37" s="3">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:16" s="3" customFormat="1">
+    <row r="38" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>2014</v>
       </c>
@@ -6904,47 +7007,50 @@
         <v>10</v>
       </c>
       <c r="C38" s="3">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D38" s="3">
+        <v>8</v>
+      </c>
+      <c r="E38" s="3">
         <v>44</v>
       </c>
-      <c r="E38" s="3">
+      <c r="F38" s="3">
         <v>2014</v>
       </c>
-      <c r="F38" s="4">
+      <c r="G38" s="4">
         <v>4</v>
       </c>
-      <c r="G38" s="4">
-        <v>1</v>
-      </c>
       <c r="H38" s="4">
+        <v>1</v>
+      </c>
+      <c r="I38" s="4">
         <v>4</v>
       </c>
-      <c r="I38" s="4">
+      <c r="J38" s="4">
         <v>8</v>
       </c>
-      <c r="J38" s="4">
+      <c r="K38" s="4">
         <v>2</v>
       </c>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4">
+      <c r="L38" s="4"/>
+      <c r="M38" s="4">
         <v>4</v>
       </c>
-      <c r="M38" s="4">
+      <c r="N38" s="4">
         <v>15</v>
       </c>
-      <c r="N38" s="4">
+      <c r="O38" s="4">
         <v>6</v>
       </c>
-      <c r="O38" s="4">
+      <c r="P38" s="4">
         <v>44</v>
       </c>
-      <c r="P38" s="3">
+      <c r="Q38" s="3">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="1:16" s="3" customFormat="1">
+    <row r="39" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>2015</v>
       </c>
@@ -6952,47 +7058,50 @@
         <v>15</v>
       </c>
       <c r="C39" s="3">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D39" s="3">
+        <v>17</v>
+      </c>
+      <c r="E39" s="3">
         <v>47</v>
       </c>
-      <c r="E39" s="3">
+      <c r="F39" s="3">
         <v>2015</v>
       </c>
-      <c r="F39" s="4">
+      <c r="G39" s="4">
         <v>5</v>
       </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4">
-        <v>1</v>
-      </c>
+      <c r="H39" s="4"/>
       <c r="I39" s="4">
+        <v>1</v>
+      </c>
+      <c r="J39" s="4">
         <v>11</v>
       </c>
-      <c r="J39" s="4">
+      <c r="K39" s="4">
         <v>6</v>
       </c>
-      <c r="K39" s="4">
+      <c r="L39" s="4">
         <v>2</v>
       </c>
-      <c r="L39" s="4">
+      <c r="M39" s="4">
         <v>4</v>
       </c>
-      <c r="M39" s="4">
+      <c r="N39" s="4">
         <v>14</v>
       </c>
-      <c r="N39" s="4">
+      <c r="O39" s="4">
         <v>4</v>
       </c>
-      <c r="O39" s="4">
+      <c r="P39" s="4">
         <v>47</v>
       </c>
-      <c r="P39" s="3">
+      <c r="Q39" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:16" s="3" customFormat="1">
+    <row r="40" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>2016</v>
       </c>
@@ -7000,49 +7109,52 @@
         <v>17</v>
       </c>
       <c r="C40" s="3">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D40" s="3">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3">
         <v>56</v>
       </c>
-      <c r="E40" s="3">
+      <c r="F40" s="3">
         <v>2016</v>
       </c>
-      <c r="F40" s="4">
+      <c r="G40" s="4">
         <v>13</v>
       </c>
-      <c r="G40" s="4">
+      <c r="H40" s="4">
         <v>3</v>
-      </c>
-      <c r="H40" s="4">
-        <v>8</v>
       </c>
       <c r="I40" s="4">
         <v>8</v>
       </c>
       <c r="J40" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K40" s="4">
         <v>1</v>
       </c>
       <c r="L40" s="4">
+        <v>1</v>
+      </c>
+      <c r="M40" s="4">
         <v>2</v>
       </c>
-      <c r="M40" s="4">
+      <c r="N40" s="4">
         <v>16</v>
       </c>
-      <c r="N40" s="4">
+      <c r="O40" s="4">
         <v>4</v>
       </c>
-      <c r="O40" s="4">
+      <c r="P40" s="4">
         <v>56</v>
       </c>
-      <c r="P40" s="3">
+      <c r="Q40" s="3">
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:16" s="3" customFormat="1">
+    <row r="41" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>2017</v>
       </c>
@@ -7050,47 +7162,50 @@
         <v>19</v>
       </c>
       <c r="C41" s="3">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D41" s="3">
+        <v>16</v>
+      </c>
+      <c r="E41" s="3">
         <v>102</v>
       </c>
-      <c r="E41" s="3">
+      <c r="F41" s="3">
         <v>2017</v>
       </c>
-      <c r="F41" s="4">
+      <c r="G41" s="4">
         <v>3</v>
       </c>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4">
+      <c r="H41" s="4"/>
+      <c r="I41" s="4">
         <v>14</v>
       </c>
-      <c r="I41" s="4">
+      <c r="J41" s="4">
         <v>24</v>
       </c>
-      <c r="J41" s="4">
+      <c r="K41" s="4">
         <v>4</v>
       </c>
-      <c r="K41" s="4">
-        <v>1</v>
-      </c>
       <c r="L41" s="4">
+        <v>1</v>
+      </c>
+      <c r="M41" s="4">
         <v>16</v>
       </c>
-      <c r="M41" s="4">
+      <c r="N41" s="4">
         <v>36</v>
       </c>
-      <c r="N41" s="4">
+      <c r="O41" s="4">
         <v>4</v>
       </c>
-      <c r="O41" s="4">
+      <c r="P41" s="4">
         <v>102</v>
       </c>
-      <c r="P41" s="3">
+      <c r="Q41" s="3">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:16" s="3" customFormat="1">
+    <row r="42" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>2018</v>
       </c>
@@ -7098,49 +7213,52 @@
         <v>36</v>
       </c>
       <c r="C42" s="3">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="D42" s="3">
+        <v>18</v>
+      </c>
+      <c r="E42" s="3">
         <v>123</v>
       </c>
-      <c r="E42" s="3">
+      <c r="F42" s="3">
         <v>2018</v>
       </c>
-      <c r="F42" s="4">
+      <c r="G42" s="4">
         <v>4</v>
       </c>
-      <c r="G42" s="4">
+      <c r="H42" s="4">
         <v>3</v>
       </c>
-      <c r="H42" s="4">
+      <c r="I42" s="4">
         <v>7</v>
       </c>
-      <c r="I42" s="4">
+      <c r="J42" s="4">
         <v>27</v>
       </c>
-      <c r="J42" s="4">
+      <c r="K42" s="4">
         <v>4</v>
       </c>
-      <c r="K42" s="4">
+      <c r="L42" s="4">
         <v>2</v>
       </c>
-      <c r="L42" s="4">
+      <c r="M42" s="4">
         <v>18</v>
       </c>
-      <c r="M42" s="4">
+      <c r="N42" s="4">
         <v>52</v>
       </c>
-      <c r="N42" s="4">
+      <c r="O42" s="4">
         <v>6</v>
       </c>
-      <c r="O42" s="4">
+      <c r="P42" s="4">
         <v>123</v>
       </c>
-      <c r="P42" s="3">
+      <c r="Q42" s="3">
         <v>123</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2019</v>
       </c>
@@ -7150,13 +7268,15 @@
       <c r="C43">
         <v>1</v>
       </c>
-      <c r="D43">
-        <v>1</v>
+      <c r="D43" s="3">
+        <v>0</v>
       </c>
       <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43">
         <v>2019</v>
       </c>
-      <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -7164,13 +7284,14 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
-      <c r="N43" s="2">
-        <v>1</v>
-      </c>
+      <c r="N43" s="2"/>
       <c r="O43" s="2">
         <v>1</v>
       </c>
-      <c r="P43">
+      <c r="P43" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q43">
         <v>1</v>
       </c>
     </row>

</xml_diff>